<commit_message>
Update requirement and implement terminal.
</commit_message>
<xml_diff>
--- a/Doc/Requirements.xlsx
+++ b/Doc/Requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Code\git\StockAnalysisSystem\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8924AFE-53E3-45F4-ABEC-B722D122B93C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908EB43D-625C-4427-BA9D-017408E2151F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,17 +17,26 @@
     <sheet name="Product Requirement - WHAT" sheetId="2" r:id="rId2"/>
     <sheet name="Feature - HOW" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="602">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -774,9 +783,6 @@
     <t>没有企业号，无法测试</t>
   </si>
   <si>
-    <t>终端服务</t>
-  </si>
-  <si>
     <t>用户可通过某种终端进行交互</t>
   </si>
   <si>
@@ -1922,6 +1928,86 @@
   </si>
   <si>
     <t>盯盘服务</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>终端服务</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>终端服务</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取分析结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>观察</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通用规则</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>股票代码不需要加上后缀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要输入股票代码的地方可以直接输入股票名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>作用：直接返回简略的分析结果和评分；同时给出完整分析结果的链接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>格式：“分析结果” + 股票代码；“分析结果”可以出现在股票代码或股票名的前面或后面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">           输入股票代码或股票名，如果正确且唯一，默认返回分析结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>格式：“观察” + 股票代码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交互命令</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>作用：将该股票加入观察列表，并将当前的价格作为基准</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置基准价格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>格式：“设置基准” + 股票代码 + 价格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>i</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>作用：为股票设置观察的价格基准；如果该股票没有加入观察列表，则自动加入观察列表；如果没有价格参数，则使用当前价格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>“+”号分隔的部分实际应以空格分隔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置通知价格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>推送</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3072,8 +3158,8 @@
   </sheetPr>
   <dimension ref="A2:H155"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="D140" sqref="D140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" outlineLevelRow="3" x14ac:dyDescent="0.25"/>
@@ -3515,7 +3601,7 @@
     </row>
     <row r="52" spans="4:8" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="F52" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>214</v>
@@ -3523,7 +3609,7 @@
     </row>
     <row r="53" spans="4:8" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="F53" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>215</v>
@@ -3537,12 +3623,12 @@
         <v>210</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="55" spans="4:8" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="F55" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>215</v>
@@ -3599,7 +3685,7 @@
     </row>
     <row r="62" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E62" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>215</v>
@@ -3607,7 +3693,7 @@
     </row>
     <row r="63" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E63" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>215</v>
@@ -3628,13 +3714,13 @@
     </row>
     <row r="66" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E66" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F66" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="F66" s="1" t="s">
+      <c r="G66" s="4" t="s">
         <v>261</v>
-      </c>
-      <c r="G66" s="4" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="67" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -3895,7 +3981,7 @@
     </row>
     <row r="117" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E117" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="118" spans="4:6" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3905,71 +3991,71 @@
     </row>
     <row r="119" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E119" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="120" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F120" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="121" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F121" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="122" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E122" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="123" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F123" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="124" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F124" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="125" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F125" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="126" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E126" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="127" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E127" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="128" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E128" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="129" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E129" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="130" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E130" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="131" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3979,53 +4065,53 @@
     </row>
     <row r="132" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E132" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="133" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E133" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="134" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D134" s="1" t="s">
-        <v>221</v>
+        <v>582</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G134" s="4"/>
     </row>
     <row r="135" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E135" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G135" s="4"/>
     </row>
     <row r="136" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E136" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G136" s="4"/>
     </row>
     <row r="137" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G137" s="4"/>
     </row>
     <row r="138" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E138" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G138" s="4"/>
     </row>
@@ -4037,25 +4123,25 @@
     </row>
     <row r="140" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F140" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G140" s="4"/>
     </row>
     <row r="141" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G141" s="4"/>
     </row>
     <row r="142" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G142" s="4"/>
     </row>
@@ -4067,13 +4153,13 @@
     </row>
     <row r="144" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F144" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G144" s="4"/>
     </row>
     <row r="145" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F145" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G145" s="4"/>
     </row>
@@ -4085,7 +4171,7 @@
     </row>
     <row r="147" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D147" s="1" t="s">
         <v>189</v>
@@ -4094,13 +4180,13 @@
     </row>
     <row r="148" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E148" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G148" s="4"/>
     </row>
     <row r="149" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E149" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G149" s="4"/>
     </row>
@@ -4112,13 +4198,13 @@
     </row>
     <row r="151" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E151" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G151" s="4"/>
     </row>
     <row r="152" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E152" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G152" s="4"/>
     </row>
@@ -4146,10 +4232,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L232"/>
+  <dimension ref="A1:L266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A215" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H232" sqref="H232"/>
+    <sheetView tabSelected="1" topLeftCell="A245" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F267" sqref="F267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -4194,7 +4280,7 @@
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
       <c r="D4" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4203,7 +4289,7 @@
       <c r="C5" s="2"/>
       <c r="D5" s="1"/>
       <c r="E5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="6" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4212,7 +4298,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="1"/>
       <c r="E6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="7" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4221,7 +4307,7 @@
       <c r="C7" s="2"/>
       <c r="D7" s="1"/>
       <c r="F7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="8" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4230,10 +4316,10 @@
       <c r="C8" s="2"/>
       <c r="D8" s="1"/>
       <c r="F8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4242,10 +4328,10 @@
       <c r="C9" s="2"/>
       <c r="D9" s="1"/>
       <c r="F9" t="s">
+        <v>383</v>
+      </c>
+      <c r="G9" t="s">
         <v>384</v>
-      </c>
-      <c r="G9" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="10" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4254,10 +4340,10 @@
       <c r="C10" s="2"/>
       <c r="D10" s="1"/>
       <c r="F10" t="s">
+        <v>385</v>
+      </c>
+      <c r="G10" t="s">
         <v>386</v>
-      </c>
-      <c r="G10" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="11" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4266,7 +4352,7 @@
       <c r="C11" s="2"/>
       <c r="D11" s="1"/>
       <c r="E11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="12" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4275,7 +4361,7 @@
       <c r="C12" s="2"/>
       <c r="D12" s="1"/>
       <c r="F12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="13" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4284,10 +4370,10 @@
       <c r="C13" s="2"/>
       <c r="D13" s="1"/>
       <c r="F13" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="14" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4296,7 +4382,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="1"/>
       <c r="E14" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="15" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4305,7 +4391,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="1"/>
       <c r="F15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="16" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4314,7 +4400,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="1"/>
       <c r="F16" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="17" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4322,7 +4408,7 @@
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
       <c r="D17" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -4330,7 +4416,7 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="19" spans="1:7" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
@@ -4339,7 +4425,7 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="20" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4348,10 +4434,10 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="F20" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G20" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="21" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4360,7 +4446,7 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="F21" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="22" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4375,7 +4461,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="F23" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="24" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4384,7 +4470,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="G24" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="25" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4393,7 +4479,7 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="G25" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="26" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4402,7 +4488,7 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="G26" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="27" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4417,7 +4503,7 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="F28" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="29" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4426,7 +4512,7 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="G29" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="30" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4435,7 +4521,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="G30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="31" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4444,7 +4530,7 @@
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="G31" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="32" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4453,7 +4539,7 @@
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="F32" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="33" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4462,7 +4548,7 @@
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="G33" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="34" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4471,7 +4557,7 @@
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="G34" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="35" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4480,7 +4566,7 @@
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="G35" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="36" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4489,58 +4575,58 @@
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="37" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="38" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="39" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F40" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G40" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H40" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I40" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J40" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="K40" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L40" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="41" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F41" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G41" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H41" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I41" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J41" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L41" t="s">
         <v>214</v>
@@ -4548,19 +4634,19 @@
     </row>
     <row r="42" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G42" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H42" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I42" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J42" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L42" t="s">
         <v>214</v>
@@ -4568,19 +4654,19 @@
     </row>
     <row r="43" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G43" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H43" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I43" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J43" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L43" t="s">
         <v>214</v>
@@ -4588,19 +4674,19 @@
     </row>
     <row r="44" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F44" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G44" t="s">
+        <v>276</v>
+      </c>
+      <c r="H44" t="s">
+        <v>310</v>
+      </c>
+      <c r="I44" t="s">
         <v>277</v>
       </c>
-      <c r="H44" t="s">
-        <v>311</v>
-      </c>
-      <c r="I44" t="s">
-        <v>278</v>
-      </c>
       <c r="J44" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L44" t="s">
         <v>215</v>
@@ -4608,19 +4694,19 @@
     </row>
     <row r="45" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F45" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G45" t="s">
+        <v>279</v>
+      </c>
+      <c r="H45" t="s">
+        <v>310</v>
+      </c>
+      <c r="I45" t="s">
         <v>280</v>
       </c>
-      <c r="H45" t="s">
-        <v>311</v>
-      </c>
-      <c r="I45" t="s">
-        <v>281</v>
-      </c>
       <c r="J45" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L45" t="s">
         <v>215</v>
@@ -4628,19 +4714,19 @@
     </row>
     <row r="46" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F46" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G46" t="s">
+        <v>281</v>
+      </c>
+      <c r="H46" t="s">
+        <v>310</v>
+      </c>
+      <c r="I46" t="s">
         <v>282</v>
       </c>
-      <c r="H46" t="s">
-        <v>311</v>
-      </c>
-      <c r="I46" t="s">
-        <v>283</v>
-      </c>
       <c r="J46" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L46" t="s">
         <v>214</v>
@@ -4648,16 +4734,16 @@
     </row>
     <row r="47" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F47" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G47" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H47" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I47" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="L47" t="s">
         <v>214</v>
@@ -4665,19 +4751,19 @@
     </row>
     <row r="48" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F48" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G48" t="s">
+        <v>284</v>
+      </c>
+      <c r="H48" t="s">
+        <v>310</v>
+      </c>
+      <c r="I48" t="s">
         <v>285</v>
       </c>
-      <c r="H48" t="s">
-        <v>311</v>
-      </c>
-      <c r="I48" t="s">
-        <v>286</v>
-      </c>
       <c r="J48" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L48" t="s">
         <v>214</v>
@@ -4685,19 +4771,19 @@
     </row>
     <row r="49" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F49" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G49" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H49" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I49" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J49" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L49" t="s">
         <v>214</v>
@@ -4705,19 +4791,19 @@
     </row>
     <row r="50" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F50" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G50" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H50" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I50" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J50" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L50" t="s">
         <v>214</v>
@@ -4725,19 +4811,19 @@
     </row>
     <row r="51" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F51" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G51" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H51" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I51" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J51" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L51" t="s">
         <v>214</v>
@@ -4745,19 +4831,19 @@
     </row>
     <row r="52" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F52" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G52" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H52" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I52" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J52" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L52" t="s">
         <v>214</v>
@@ -4765,19 +4851,19 @@
     </row>
     <row r="53" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F53" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G53" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H53" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I53" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J53" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L53" t="s">
         <v>214</v>
@@ -4785,16 +4871,16 @@
     </row>
     <row r="54" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F54" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G54" t="s">
+        <v>293</v>
+      </c>
+      <c r="H54" t="s">
+        <v>310</v>
+      </c>
+      <c r="I54" t="s">
         <v>294</v>
-      </c>
-      <c r="H54" t="s">
-        <v>311</v>
-      </c>
-      <c r="I54" t="s">
-        <v>295</v>
       </c>
       <c r="L54" t="s">
         <v>214</v>
@@ -4802,16 +4888,16 @@
     </row>
     <row r="55" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F55" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G55" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H55" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I55" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L55" t="s">
         <v>214</v>
@@ -4819,16 +4905,16 @@
     </row>
     <row r="56" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F56" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G56" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H56" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I56" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L56" t="s">
         <v>214</v>
@@ -4836,19 +4922,19 @@
     </row>
     <row r="57" spans="6:12" ht="27.6" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F57" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G57" t="s">
+        <v>298</v>
+      </c>
+      <c r="H57" t="s">
+        <v>311</v>
+      </c>
+      <c r="I57" t="s">
         <v>299</v>
       </c>
-      <c r="H57" t="s">
-        <v>312</v>
-      </c>
-      <c r="I57" t="s">
-        <v>300</v>
-      </c>
       <c r="K57" s="7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="L57" t="s">
         <v>214</v>
@@ -4856,19 +4942,19 @@
     </row>
     <row r="58" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F58" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G58" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H58" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I58" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J58" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L58" t="s">
         <v>214</v>
@@ -4876,19 +4962,19 @@
     </row>
     <row r="59" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F59" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G59" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H59" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I59" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J59" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L59" t="s">
         <v>214</v>
@@ -4896,19 +4982,19 @@
     </row>
     <row r="60" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F60" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G60" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H60" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I60" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J60" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L60" t="s">
         <v>214</v>
@@ -4916,16 +5002,16 @@
     </row>
     <row r="61" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F61" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G61" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H61" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I61" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L61" t="s">
         <v>214</v>
@@ -4933,16 +5019,16 @@
     </row>
     <row r="62" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F62" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G62" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H62" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I62" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L62" t="s">
         <v>214</v>
@@ -4950,16 +5036,16 @@
     </row>
     <row r="63" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F63" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G63" t="s">
+        <v>305</v>
+      </c>
+      <c r="H63" t="s">
+        <v>310</v>
+      </c>
+      <c r="I63" t="s">
         <v>306</v>
-      </c>
-      <c r="H63" t="s">
-        <v>311</v>
-      </c>
-      <c r="I63" t="s">
-        <v>307</v>
       </c>
       <c r="L63" t="s">
         <v>214</v>
@@ -4968,245 +5054,245 @@
     <row r="64" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25"/>
     <row r="65" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F65" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G65" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="H65" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I65" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="J65" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L65" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="66" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F66" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="G66" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="H66" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I66" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="J66" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L66" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="67" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F67" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G67" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H67" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I67" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="J67" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L67" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="68" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F68" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G68" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="H68" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I68" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="L68" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="69" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25"/>
     <row r="70" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F70" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G70" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H70" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I70" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="J70" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L70" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="71" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F71" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G71" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="H71" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I71" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="J71" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L71" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="72" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F72" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G72" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H72" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I72" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="J72" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L72" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="73" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F73" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G73" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H73" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I73" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="J73" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L73" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="74" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F74" t="s">
+        <v>548</v>
+      </c>
+      <c r="G74" t="s">
         <v>549</v>
       </c>
-      <c r="G74" t="s">
-        <v>550</v>
-      </c>
       <c r="H74" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I74" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="J74" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L74" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="75" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F75" t="s">
+        <v>550</v>
+      </c>
+      <c r="G75" t="s">
         <v>551</v>
       </c>
-      <c r="G75" t="s">
+      <c r="H75" t="s">
+        <v>310</v>
+      </c>
+      <c r="I75" t="s">
         <v>552</v>
       </c>
-      <c r="H75" t="s">
-        <v>311</v>
-      </c>
-      <c r="I75" t="s">
-        <v>553</v>
-      </c>
       <c r="J75" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L75" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="76" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25"/>
     <row r="77" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E77" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="78" spans="5:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="E78" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="79" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F79" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="80" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25"/>
     <row r="81" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G81" t="s">
+        <v>265</v>
+      </c>
+      <c r="H81" t="s">
         <v>266</v>
       </c>
-      <c r="H81" t="s">
-        <v>267</v>
-      </c>
       <c r="I81" t="s">
+        <v>337</v>
+      </c>
+      <c r="J81" t="s">
         <v>338</v>
       </c>
-      <c r="J81" t="s">
-        <v>339</v>
-      </c>
       <c r="K81" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="82" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G82" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H82" t="s">
+        <v>263</v>
+      </c>
+      <c r="I82" s="5" t="s">
         <v>264</v>
-      </c>
-      <c r="I82" s="5" t="s">
-        <v>265</v>
       </c>
       <c r="K82" t="s">
         <v>214</v>
@@ -5214,13 +5300,13 @@
     </row>
     <row r="83" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G83" t="s">
+        <v>269</v>
+      </c>
+      <c r="H83" t="s">
         <v>270</v>
       </c>
-      <c r="H83" t="s">
-        <v>271</v>
-      </c>
       <c r="I83" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="K83" t="s">
         <v>214</v>
@@ -5228,13 +5314,13 @@
     </row>
     <row r="84" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G84" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H84" t="s">
+        <v>339</v>
+      </c>
+      <c r="I84" s="5" t="s">
         <v>340</v>
-      </c>
-      <c r="I84" s="5" t="s">
-        <v>341</v>
       </c>
       <c r="K84" t="s">
         <v>214</v>
@@ -5242,13 +5328,13 @@
     </row>
     <row r="85" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G85" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H85" t="s">
+        <v>341</v>
+      </c>
+      <c r="I85" s="5" t="s">
         <v>342</v>
-      </c>
-      <c r="I85" s="5" t="s">
-        <v>343</v>
       </c>
       <c r="K85" t="s">
         <v>214</v>
@@ -5256,13 +5342,13 @@
     </row>
     <row r="86" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G86" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H86" t="s">
+        <v>360</v>
+      </c>
+      <c r="I86" s="5" t="s">
         <v>361</v>
-      </c>
-      <c r="I86" s="5" t="s">
-        <v>362</v>
       </c>
       <c r="K86" t="s">
         <v>214</v>
@@ -5270,13 +5356,13 @@
     </row>
     <row r="87" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G87" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H87" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I87" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K87" t="s">
         <v>214</v>
@@ -5284,13 +5370,13 @@
     </row>
     <row r="88" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G88" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H88" t="s">
+        <v>347</v>
+      </c>
+      <c r="I88" s="5" t="s">
         <v>348</v>
-      </c>
-      <c r="I88" s="5" t="s">
-        <v>349</v>
       </c>
       <c r="K88" t="s">
         <v>214</v>
@@ -5298,13 +5384,13 @@
     </row>
     <row r="89" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G89" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H89" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I89" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K89" t="s">
         <v>214</v>
@@ -5312,13 +5398,13 @@
     </row>
     <row r="90" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G90" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H90" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I90" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K90" t="s">
         <v>214</v>
@@ -5326,13 +5412,13 @@
     </row>
     <row r="91" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G91" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H91" t="s">
+        <v>352</v>
+      </c>
+      <c r="I91" s="5" t="s">
         <v>353</v>
-      </c>
-      <c r="I91" s="5" t="s">
-        <v>354</v>
       </c>
       <c r="K91" t="s">
         <v>214</v>
@@ -5340,13 +5426,13 @@
     </row>
     <row r="92" spans="7:11" ht="41.4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G92" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H92" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="I92" s="6" t="s">
         <v>359</v>
-      </c>
-      <c r="I92" s="6" t="s">
-        <v>360</v>
       </c>
       <c r="K92" t="s">
         <v>214</v>
@@ -5354,13 +5440,13 @@
     </row>
     <row r="93" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G93" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H93" t="s">
+        <v>362</v>
+      </c>
+      <c r="I93" s="5" t="s">
         <v>363</v>
-      </c>
-      <c r="I93" s="5" t="s">
-        <v>364</v>
       </c>
       <c r="K93" t="s">
         <v>214</v>
@@ -5368,13 +5454,13 @@
     </row>
     <row r="94" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G94" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H94" t="s">
+        <v>364</v>
+      </c>
+      <c r="I94" s="5" t="s">
         <v>365</v>
-      </c>
-      <c r="I94" s="5" t="s">
-        <v>366</v>
       </c>
       <c r="K94" t="s">
         <v>214</v>
@@ -5382,13 +5468,13 @@
     </row>
     <row r="95" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G95" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H95" t="s">
+        <v>366</v>
+      </c>
+      <c r="I95" s="5" t="s">
         <v>367</v>
-      </c>
-      <c r="I95" s="5" t="s">
-        <v>368</v>
       </c>
       <c r="K95" t="s">
         <v>214</v>
@@ -5396,13 +5482,13 @@
     </row>
     <row r="96" spans="7:11" ht="27.6" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G96" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H96" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I96" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="K96" t="s">
         <v>214</v>
@@ -5410,13 +5496,13 @@
     </row>
     <row r="97" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G97" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H97" t="s">
+        <v>368</v>
+      </c>
+      <c r="I97" s="5" t="s">
         <v>369</v>
-      </c>
-      <c r="I97" s="5" t="s">
-        <v>370</v>
       </c>
       <c r="K97" t="s">
         <v>214</v>
@@ -5424,13 +5510,13 @@
     </row>
     <row r="98" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G98" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H98" t="s">
+        <v>370</v>
+      </c>
+      <c r="I98" s="5" t="s">
         <v>371</v>
-      </c>
-      <c r="I98" s="5" t="s">
-        <v>372</v>
       </c>
       <c r="K98" t="s">
         <v>214</v>
@@ -5438,13 +5524,13 @@
     </row>
     <row r="99" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G99" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H99" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I99" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="K99" t="s">
         <v>214</v>
@@ -5452,13 +5538,13 @@
     </row>
     <row r="100" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G100" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H100" t="s">
+        <v>373</v>
+      </c>
+      <c r="I100" s="5" t="s">
         <v>374</v>
-      </c>
-      <c r="I100" s="5" t="s">
-        <v>375</v>
       </c>
       <c r="K100" t="s">
         <v>214</v>
@@ -5469,58 +5555,58 @@
     </row>
     <row r="102" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G102" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="H102" t="s">
+        <v>565</v>
+      </c>
+      <c r="I102" s="5" t="s">
         <v>566</v>
       </c>
-      <c r="I102" s="5" t="s">
-        <v>567</v>
-      </c>
       <c r="K102" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="103" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G103" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="H103" t="s">
+        <v>567</v>
+      </c>
+      <c r="I103" s="5" t="s">
         <v>568</v>
       </c>
-      <c r="I103" s="5" t="s">
-        <v>569</v>
-      </c>
       <c r="K103" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="104" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G104" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H104" t="s">
+        <v>569</v>
+      </c>
+      <c r="I104" s="5" t="s">
         <v>570</v>
       </c>
-      <c r="I104" s="5" t="s">
-        <v>571</v>
-      </c>
       <c r="K104" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="105" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G105" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="H105" t="s">
+        <v>571</v>
+      </c>
+      <c r="I105" s="5" t="s">
         <v>572</v>
       </c>
-      <c r="I105" s="5" t="s">
+      <c r="K105" t="s">
         <v>573</v>
-      </c>
-      <c r="K105" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="106" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5528,86 +5614,86 @@
     </row>
     <row r="107" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G107" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H107" t="s">
+        <v>553</v>
+      </c>
+      <c r="I107" s="5" t="s">
         <v>554</v>
       </c>
-      <c r="I107" s="5" t="s">
-        <v>555</v>
-      </c>
       <c r="K107" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="108" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G108" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="H108" t="s">
+        <v>555</v>
+      </c>
+      <c r="I108" s="5" t="s">
         <v>556</v>
       </c>
-      <c r="I108" s="5" t="s">
-        <v>557</v>
-      </c>
       <c r="K108" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="109" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G109" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H109" t="s">
+        <v>557</v>
+      </c>
+      <c r="I109" s="5" t="s">
         <v>558</v>
       </c>
-      <c r="I109" s="5" t="s">
-        <v>559</v>
-      </c>
       <c r="K109" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="110" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G110" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H110" t="s">
+        <v>559</v>
+      </c>
+      <c r="I110" s="5" t="s">
         <v>560</v>
       </c>
-      <c r="I110" s="5" t="s">
-        <v>561</v>
-      </c>
       <c r="K110" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="111" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G111" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H111" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I111" s="5" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="K111" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="112" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G112" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="H112" t="s">
+        <v>563</v>
+      </c>
+      <c r="I112" s="5" t="s">
         <v>564</v>
       </c>
-      <c r="I112" s="5" t="s">
-        <v>565</v>
-      </c>
       <c r="K112" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="113" spans="4:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5615,50 +5701,50 @@
     </row>
     <row r="114" spans="4:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F114" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I114" s="5"/>
       <c r="K114" s="8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="115" spans="4:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E115" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="116" spans="4:11" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="E116" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="117" spans="4:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E117" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="118" spans="4:11" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="E118" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="119" spans="4:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G119" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H119" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K119" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="120" spans="4:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G120" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H120" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="K120" t="s">
         <v>215</v>
@@ -5666,13 +5752,13 @@
     </row>
     <row r="121" spans="4:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E121" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G121" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H121" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="K121" t="s">
         <v>215</v>
@@ -5681,131 +5767,131 @@
     <row r="122" spans="4:11" outlineLevel="1" x14ac:dyDescent="0.25"/>
     <row r="123" spans="4:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D123" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="124" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D124" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="125" spans="4:11" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="E125" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="126" spans="4:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F126" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G126" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="127" spans="4:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F127" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="128" spans="4:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25"/>
     <row r="129" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F129" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="130" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G130" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="131" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G131" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="132" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G132" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H132" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="133" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G133" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H133" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="134" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G134" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H134" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="135" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G135" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H135" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="136" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G136" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H136" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="137" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G137" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H137" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="138" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G138" t="s">
+        <v>432</v>
+      </c>
+      <c r="H138" t="s">
         <v>433</v>
-      </c>
-      <c r="H138" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="139" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="G139" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="140" spans="5:9" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="E140" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="141" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F141" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H141" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I141" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="142" spans="5:9" ht="55.2" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F142" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H142" s="7" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I142" t="s">
         <v>214</v>
@@ -5813,10 +5899,10 @@
     </row>
     <row r="143" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F143" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H143" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I143" t="s">
         <v>214</v>
@@ -5824,7 +5910,7 @@
     </row>
     <row r="144" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F144" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I144" t="s">
         <v>214</v>
@@ -5832,10 +5918,10 @@
     </row>
     <row r="145" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F145" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H145" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="I145" t="s">
         <v>214</v>
@@ -5843,10 +5929,10 @@
     </row>
     <row r="146" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F146" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H146" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I146" t="s">
         <v>214</v>
@@ -5854,10 +5940,10 @@
     </row>
     <row r="147" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F147" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H147" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I147" t="s">
         <v>214</v>
@@ -5865,7 +5951,7 @@
     </row>
     <row r="148" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F148" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="I148" t="s">
         <v>214</v>
@@ -5873,7 +5959,7 @@
     </row>
     <row r="149" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F149" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="I149" t="s">
         <v>214</v>
@@ -5881,7 +5967,7 @@
     </row>
     <row r="150" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F150" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="I150" t="s">
         <v>214</v>
@@ -5889,7 +5975,7 @@
     </row>
     <row r="151" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F151" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="I151" t="s">
         <v>214</v>
@@ -5897,7 +5983,7 @@
     </row>
     <row r="152" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F152" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I152" t="s">
         <v>214</v>
@@ -5905,7 +5991,7 @@
     </row>
     <row r="153" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F153" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="I153" t="s">
         <v>214</v>
@@ -5913,7 +5999,7 @@
     </row>
     <row r="154" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F154" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="I154" t="s">
         <v>214</v>
@@ -5921,7 +6007,7 @@
     </row>
     <row r="155" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F155" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I155" t="s">
         <v>214</v>
@@ -5929,7 +6015,7 @@
     </row>
     <row r="156" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F156" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I156" t="s">
         <v>214</v>
@@ -5937,7 +6023,7 @@
     </row>
     <row r="157" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F157" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I157" t="s">
         <v>214</v>
@@ -5945,7 +6031,7 @@
     </row>
     <row r="158" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F158" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I158" t="s">
         <v>214</v>
@@ -5953,7 +6039,7 @@
     </row>
     <row r="159" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F159" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I159" t="s">
         <v>214</v>
@@ -5961,7 +6047,7 @@
     </row>
     <row r="160" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F160" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I160" t="s">
         <v>214</v>
@@ -5969,7 +6055,7 @@
     </row>
     <row r="161" spans="4:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F161" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I161" t="s">
         <v>215</v>
@@ -5977,7 +6063,7 @@
     </row>
     <row r="162" spans="4:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F162" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="I162" t="s">
         <v>215</v>
@@ -5985,7 +6071,7 @@
     </row>
     <row r="163" spans="4:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F163" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I163" t="s">
         <v>215</v>
@@ -5993,10 +6079,10 @@
     </row>
     <row r="164" spans="4:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F164" t="s">
+        <v>461</v>
+      </c>
+      <c r="H164" t="s">
         <v>462</v>
-      </c>
-      <c r="H164" t="s">
-        <v>463</v>
       </c>
       <c r="I164" t="s">
         <v>215</v>
@@ -6005,13 +6091,13 @@
     <row r="165" spans="4:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25"/>
     <row r="166" spans="4:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="E166" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="167" spans="4:9" outlineLevel="1" x14ac:dyDescent="0.25"/>
     <row r="168" spans="4:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D168" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="169" spans="4:9" x14ac:dyDescent="0.25">
@@ -6021,331 +6107,426 @@
     </row>
     <row r="170" spans="4:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="E170" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="171" spans="4:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="F171" t="s">
+        <v>471</v>
+      </c>
+      <c r="G171" t="s">
         <v>472</v>
-      </c>
-      <c r="G171" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="172" spans="4:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="F172" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="173" spans="4:9" outlineLevel="1" x14ac:dyDescent="0.25"/>
     <row r="174" spans="4:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="F174" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="175" spans="4:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="G175" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="176" spans="4:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="G176" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="177" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="G177" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H177" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="178" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="G178" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="H178" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="179" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="G179" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H179" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="180" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="G180" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="H180" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="181" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="G181" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H181" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="182" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="G182" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H182" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="183" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="G183" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="H183" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="184" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="G184" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H184" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="185" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="G185" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="186" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25"/>
     <row r="187" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="E187" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="188" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="F188" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="189" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="F189" s="7"/>
       <c r="G189" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="190" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="F190" s="7"/>
       <c r="G190" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="191" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="F191" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="192" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="F192" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="193" spans="5:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="F193" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="194" spans="5:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="F194" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="195" spans="5:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="E195" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="196" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F196" t="s">
+        <v>491</v>
+      </c>
+      <c r="G196" t="s">
         <v>492</v>
-      </c>
-      <c r="G196" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="197" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F197" t="s">
+        <v>489</v>
+      </c>
+      <c r="G197" t="s">
         <v>490</v>
-      </c>
-      <c r="G197" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="198" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F198" t="s">
+        <v>493</v>
+      </c>
+      <c r="G198" t="s">
         <v>494</v>
-      </c>
-      <c r="G198" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="199" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25"/>
     <row r="200" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F200" t="s">
+        <v>495</v>
+      </c>
+      <c r="G200" t="s">
         <v>496</v>
-      </c>
-      <c r="G200" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="201" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F201" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G201" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="202" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F202" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="G202" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="203" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F203" t="s">
+        <v>501</v>
+      </c>
+      <c r="G203" t="s">
         <v>502</v>
-      </c>
-      <c r="G203" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="204" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F204" t="s">
+        <v>503</v>
+      </c>
+      <c r="G204" t="s">
         <v>504</v>
-      </c>
-      <c r="G204" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="205" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F205" t="s">
+        <v>505</v>
+      </c>
+      <c r="G205" t="s">
         <v>506</v>
-      </c>
-      <c r="G205" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="206" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F206" t="s">
+        <v>507</v>
+      </c>
+      <c r="G206" t="s">
         <v>508</v>
-      </c>
-      <c r="G206" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="207" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F207" t="s">
+        <v>509</v>
+      </c>
+      <c r="G207" t="s">
         <v>510</v>
-      </c>
-      <c r="G207" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="208" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25"/>
     <row r="209" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F209" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G209" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="210" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F210" t="s">
+        <v>512</v>
+      </c>
+      <c r="G210" t="s">
         <v>513</v>
-      </c>
-      <c r="G210" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="211" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F211" t="s">
+        <v>515</v>
+      </c>
+      <c r="G211" t="s">
         <v>516</v>
-      </c>
-      <c r="G211" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="212" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F212" t="s">
+        <v>517</v>
+      </c>
+      <c r="G212" t="s">
         <v>518</v>
-      </c>
-      <c r="G212" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="213" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F213" t="s">
+        <v>519</v>
+      </c>
+      <c r="G213" t="s">
         <v>520</v>
-      </c>
-      <c r="G213" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="214" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F214" t="s">
+        <v>521</v>
+      </c>
+      <c r="G214" t="s">
         <v>522</v>
-      </c>
-      <c r="G214" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="215" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="F215" t="s">
+        <v>523</v>
+      </c>
+      <c r="G215" t="s">
         <v>524</v>
-      </c>
-      <c r="G215" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="216" spans="4:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="E216" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="217" spans="4:7" outlineLevel="1" x14ac:dyDescent="0.25"/>
     <row r="218" spans="4:7" outlineLevel="1" x14ac:dyDescent="0.25"/>
     <row r="219" spans="4:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D219" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="221" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D221" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="222" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F222" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="227" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F227" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="232" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F232" t="s">
-        <v>582</v>
+        <v>581</v>
+      </c>
+    </row>
+    <row r="242" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D242" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="243" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E243" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="244" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F244" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="245" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F245" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="246" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F246" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="247" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E247" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="248" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F248" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="249" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="G249" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="250" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="G250" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="251" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="G251" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="253" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F253" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="254" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="G254" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="255" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="G255" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F259" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G260" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G261" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F263" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E266" t="s">
+        <v>601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stash updating terminal service.
Change-Id: I53a191e8381b1fed5e2a07e1199f334e929375e4
</commit_message>
<xml_diff>
--- a/Doc/Requirements.xlsx
+++ b/Doc/Requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Code\git\StockAnalysisSystem\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Private\Code\git\StockAnalysisSystem\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908EB43D-625C-4427-BA9D-017408E2151F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F0CFC0-1A09-4CC4-BC48-227790E8577D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Requirement - WHY" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="605">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2010,22 +2009,31 @@
     <t>推送</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>支持项目</t>
+  </si>
+  <si>
+    <t>格式："支持" "打赏" "捐助"</t>
+  </si>
+  <si>
+    <t>作用：发送微信收款码</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2034,7 +2042,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2090,8 +2098,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2378,20 +2386,20 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
-    <col min="2" max="2" width="7.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="91.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="7.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="91.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2414,7 +2422,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" ht="30">
       <c r="C3" s="2" t="s">
         <v>53</v>
       </c>
@@ -2425,7 +2433,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" outlineLevel="1">
       <c r="D4" s="1" t="s">
         <v>27</v>
       </c>
@@ -2434,7 +2442,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="55.2" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="60" outlineLevel="2">
       <c r="E5" s="1" t="s">
         <v>1</v>
       </c>
@@ -2445,7 +2453,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="2:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" outlineLevel="2">
       <c r="E6" s="1" t="s">
         <v>23</v>
       </c>
@@ -2454,7 +2462,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="27.6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="30" outlineLevel="2">
       <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
@@ -2465,7 +2473,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="8" spans="2:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" outlineLevel="2">
       <c r="E8" s="1" t="s">
         <v>4</v>
       </c>
@@ -2476,7 +2484,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="2:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" outlineLevel="2">
       <c r="E9" s="1" t="s">
         <v>2</v>
       </c>
@@ -2487,7 +2495,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="2:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" outlineLevel="2">
       <c r="E10" s="1" t="s">
         <v>5</v>
       </c>
@@ -2495,7 +2503,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" outlineLevel="1">
       <c r="D11" s="1" t="s">
         <v>28</v>
       </c>
@@ -2503,7 +2511,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="27.6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" ht="30" outlineLevel="2">
       <c r="E12" s="1" t="s">
         <v>3</v>
       </c>
@@ -2514,7 +2522,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="2:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" outlineLevel="2">
       <c r="E13" s="1" t="s">
         <v>25</v>
       </c>
@@ -2522,7 +2530,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="14" spans="2:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" outlineLevel="2">
       <c r="E14" s="1" t="s">
         <v>26</v>
       </c>
@@ -2530,7 +2538,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" outlineLevel="1">
       <c r="D15" s="1" t="s">
         <v>31</v>
       </c>
@@ -2538,7 +2546,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="16" spans="2:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" outlineLevel="2">
       <c r="E16" s="1" t="s">
         <v>49</v>
       </c>
@@ -2546,7 +2554,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="17" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:7" outlineLevel="2">
       <c r="E17" s="1" t="s">
         <v>6</v>
       </c>
@@ -2554,7 +2562,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="18" spans="4:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:7" outlineLevel="1">
       <c r="D18" s="1" t="s">
         <v>32</v>
       </c>
@@ -2562,7 +2570,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:7" outlineLevel="2">
       <c r="E19" s="1" t="s">
         <v>41</v>
       </c>
@@ -2570,7 +2578,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="20" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:7" outlineLevel="2">
       <c r="E20" s="1" t="s">
         <v>40</v>
       </c>
@@ -2578,7 +2586,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="21" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:7" outlineLevel="2">
       <c r="E21" s="1" t="s">
         <v>35</v>
       </c>
@@ -2586,7 +2594,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="22" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:7" outlineLevel="2">
       <c r="E22" s="1" t="s">
         <v>36</v>
       </c>
@@ -2594,7 +2602,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="23" spans="4:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:7" outlineLevel="1">
       <c r="D23" s="1" t="s">
         <v>33</v>
       </c>
@@ -2602,7 +2610,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="24" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:7" outlineLevel="2">
       <c r="E24" s="1" t="s">
         <v>34</v>
       </c>
@@ -2610,7 +2618,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="25" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:7" outlineLevel="2">
       <c r="E25" s="1" t="s">
         <v>37</v>
       </c>
@@ -2618,7 +2626,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="26" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:7" outlineLevel="2">
       <c r="E26" s="1" t="s">
         <v>7</v>
       </c>
@@ -2626,7 +2634,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="27" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:7" outlineLevel="2">
       <c r="E27" s="1" t="s">
         <v>8</v>
       </c>
@@ -2634,7 +2642,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="28" spans="4:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:7" outlineLevel="1">
       <c r="D28" s="1" t="s">
         <v>118</v>
       </c>
@@ -2642,7 +2650,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="29" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:7" outlineLevel="2">
       <c r="E29" s="1" t="s">
         <v>117</v>
       </c>
@@ -2650,7 +2658,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="30" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:7" outlineLevel="2">
       <c r="E30" s="1" t="s">
         <v>119</v>
       </c>
@@ -2658,7 +2666,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="31" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:7" outlineLevel="2">
       <c r="E31" s="1" t="s">
         <v>120</v>
       </c>
@@ -2666,7 +2674,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="32" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:7" outlineLevel="2">
       <c r="E32" s="1" t="s">
         <v>121</v>
       </c>
@@ -2674,7 +2682,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="33" spans="3:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:8" outlineLevel="1">
       <c r="D33" s="1" t="s">
         <v>38</v>
       </c>
@@ -2682,7 +2690,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="34" spans="3:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:8" outlineLevel="2">
       <c r="E34" s="1" t="s">
         <v>11</v>
       </c>
@@ -2693,7 +2701,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="35" spans="3:8" ht="27.6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:8" ht="30" outlineLevel="2">
       <c r="E35" s="1" t="s">
         <v>9</v>
       </c>
@@ -2707,7 +2715,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="36" spans="3:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:8" outlineLevel="2">
       <c r="E36" s="1" t="s">
         <v>10</v>
       </c>
@@ -2721,7 +2729,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="37" spans="3:8" ht="55.2" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:8" ht="60" outlineLevel="2">
       <c r="E37" s="1" t="s">
         <v>12</v>
       </c>
@@ -2735,7 +2743,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="38" spans="3:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:8" outlineLevel="1">
       <c r="D38" s="1" t="s">
         <v>44</v>
       </c>
@@ -2743,7 +2751,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="39" spans="3:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:8" outlineLevel="2">
       <c r="E39" s="1" t="s">
         <v>48</v>
       </c>
@@ -2751,7 +2759,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="40" spans="3:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:8" outlineLevel="2">
       <c r="E40" s="1" t="s">
         <v>50</v>
       </c>
@@ -2759,7 +2767,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="41" spans="3:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:8" outlineLevel="2">
       <c r="E41" s="1" t="s">
         <v>52</v>
       </c>
@@ -2767,7 +2775,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="42" spans="3:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:8" outlineLevel="2">
       <c r="E42" s="1" t="s">
         <v>45</v>
       </c>
@@ -2775,7 +2783,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="43" spans="3:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:8" outlineLevel="2">
       <c r="E43" s="1" t="s">
         <v>46</v>
       </c>
@@ -2783,7 +2791,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="44" spans="3:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:8" outlineLevel="2">
       <c r="E44" s="1" t="s">
         <v>47</v>
       </c>
@@ -2791,7 +2799,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="45" spans="3:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:8" outlineLevel="1">
       <c r="C45" s="3" t="s">
         <v>55</v>
       </c>
@@ -2799,7 +2807,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:8">
       <c r="C46" s="1" t="s">
         <v>51</v>
       </c>
@@ -2807,7 +2815,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="47" spans="3:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:8" outlineLevel="1">
       <c r="D47" s="1" t="s">
         <v>54</v>
       </c>
@@ -2815,7 +2823,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="48" spans="3:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:8" outlineLevel="2">
       <c r="E48" s="1" t="s">
         <v>13</v>
       </c>
@@ -2823,7 +2831,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="49" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:7" outlineLevel="2">
       <c r="E49" s="1" t="s">
         <v>14</v>
       </c>
@@ -2831,7 +2839,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="50" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:7" outlineLevel="2">
       <c r="E50" s="1" t="s">
         <v>15</v>
       </c>
@@ -2839,7 +2847,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="51" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:7" outlineLevel="2">
       <c r="E51" s="1" t="s">
         <v>59</v>
       </c>
@@ -2847,7 +2855,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="52" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:7" outlineLevel="2">
       <c r="E52" s="1" t="s">
         <v>57</v>
       </c>
@@ -2855,7 +2863,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="53" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:7" outlineLevel="2">
       <c r="E53" s="1" t="s">
         <v>56</v>
       </c>
@@ -2863,7 +2871,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="54" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:7" outlineLevel="2">
       <c r="E54" s="1" t="s">
         <v>60</v>
       </c>
@@ -2871,12 +2879,12 @@
         <v>214</v>
       </c>
     </row>
-    <row r="55" spans="4:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:7" outlineLevel="1">
       <c r="D55" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="56" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:7" outlineLevel="2">
       <c r="E56" s="1" t="s">
         <v>181</v>
       </c>
@@ -2884,7 +2892,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="57" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:7" outlineLevel="2">
       <c r="E57" s="1" t="s">
         <v>16</v>
       </c>
@@ -2892,7 +2900,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="58" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:7" outlineLevel="2">
       <c r="E58" s="1" t="s">
         <v>17</v>
       </c>
@@ -2900,7 +2908,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="4:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:7" outlineLevel="1">
       <c r="D59" s="1" t="s">
         <v>58</v>
       </c>
@@ -2908,7 +2916,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="60" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:7" outlineLevel="2">
       <c r="E60" s="1" t="s">
         <v>61</v>
       </c>
@@ -2916,7 +2924,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="61" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:7" outlineLevel="2">
       <c r="E61" s="1" t="s">
         <v>63</v>
       </c>
@@ -2924,7 +2932,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="62" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:7" outlineLevel="2">
       <c r="E62" s="1" t="s">
         <v>62</v>
       </c>
@@ -2932,7 +2940,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="63" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:7" outlineLevel="2">
       <c r="E63" s="1" t="s">
         <v>64</v>
       </c>
@@ -2940,7 +2948,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="64" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:7" outlineLevel="2">
       <c r="E64" s="1" t="s">
         <v>65</v>
       </c>
@@ -2948,7 +2956,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="4:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:8" outlineLevel="1">
       <c r="D65" s="1" t="s">
         <v>66</v>
       </c>
@@ -2956,7 +2964,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="66" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:8" outlineLevel="2">
       <c r="E66" s="1" t="s">
         <v>188</v>
       </c>
@@ -2967,7 +2975,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="67" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:8" outlineLevel="2">
       <c r="E67" s="1" t="s">
         <v>67</v>
       </c>
@@ -2975,7 +2983,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="68" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:8" outlineLevel="2">
       <c r="E68" s="1" t="s">
         <v>182</v>
       </c>
@@ -2983,7 +2991,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="69" spans="4:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:8" outlineLevel="1">
       <c r="D69" s="1" t="s">
         <v>189</v>
       </c>
@@ -2991,7 +2999,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="70" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:8" outlineLevel="2">
       <c r="E70" s="1" t="s">
         <v>191</v>
       </c>
@@ -3002,7 +3010,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="71" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:8" outlineLevel="2">
       <c r="E71" s="1" t="s">
         <v>198</v>
       </c>
@@ -3010,7 +3018,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="72" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:8" outlineLevel="2">
       <c r="E72" s="1" t="s">
         <v>194</v>
       </c>
@@ -3018,7 +3026,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="73" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:8" outlineLevel="2">
       <c r="E73" s="1" t="s">
         <v>195</v>
       </c>
@@ -3026,7 +3034,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="74" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:8" outlineLevel="2">
       <c r="F74" s="1" t="s">
         <v>197</v>
       </c>
@@ -3034,7 +3042,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="75" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:8" outlineLevel="2">
       <c r="F75" s="1" t="s">
         <v>203</v>
       </c>
@@ -3042,7 +3050,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="76" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:8" outlineLevel="2">
       <c r="F76" s="1" t="s">
         <v>202</v>
       </c>
@@ -3050,7 +3058,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="77" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:8" outlineLevel="2">
       <c r="E77" s="1" t="s">
         <v>196</v>
       </c>
@@ -3058,7 +3066,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="78" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:8" outlineLevel="2">
       <c r="F78" s="1" t="s">
         <v>199</v>
       </c>
@@ -3066,7 +3074,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="79" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:8" outlineLevel="2">
       <c r="F79" s="1" t="s">
         <v>200</v>
       </c>
@@ -3074,7 +3082,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="80" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:8" outlineLevel="2">
       <c r="F80" s="1" t="s">
         <v>201</v>
       </c>
@@ -3082,7 +3090,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="81" spans="3:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:8" outlineLevel="2">
       <c r="F81" s="1" t="s">
         <v>204</v>
       </c>
@@ -3090,12 +3098,12 @@
         <v>215</v>
       </c>
     </row>
-    <row r="82" spans="3:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:8" outlineLevel="1">
       <c r="D82" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="83" spans="3:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:8" outlineLevel="2">
       <c r="E83" s="1" t="s">
         <v>192</v>
       </c>
@@ -3103,7 +3111,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="84" spans="3:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:8" outlineLevel="2">
       <c r="E84" s="1" t="s">
         <v>218</v>
       </c>
@@ -3111,7 +3119,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="85" spans="3:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:8" outlineLevel="2">
       <c r="E85" s="1" t="s">
         <v>219</v>
       </c>
@@ -3122,7 +3130,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="86" spans="3:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:8" outlineLevel="2">
       <c r="E86" s="1" t="s">
         <v>194</v>
       </c>
@@ -3130,7 +3138,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="87" spans="3:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:8" outlineLevel="2">
       <c r="E87" s="1" t="s">
         <v>205</v>
       </c>
@@ -3138,8 +3146,8 @@
         <v>210</v>
       </c>
     </row>
-    <row r="88" spans="3:8" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="89" spans="3:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:8" outlineLevel="1"/>
+    <row r="89" spans="3:8" outlineLevel="1">
       <c r="C89" s="3" t="s">
         <v>55</v>
       </c>
@@ -3162,19 +3170,19 @@
       <selection activeCell="D140" sqref="D140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" outlineLevelRow="3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="79.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="79.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="104" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="67.5546875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="1"/>
+    <col min="7" max="7" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="67.5703125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3185,7 +3193,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8">
       <c r="C3" s="2" t="s">
         <v>53</v>
       </c>
@@ -3193,7 +3201,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" outlineLevel="1">
       <c r="D4" s="1" t="s">
         <v>72</v>
       </c>
@@ -3201,7 +3209,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="2:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" outlineLevel="2">
       <c r="E5" s="1" t="s">
         <v>69</v>
       </c>
@@ -3212,7 +3220,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="2:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" outlineLevel="2">
       <c r="E6" s="1" t="s">
         <v>74</v>
       </c>
@@ -3223,7 +3231,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="7" spans="2:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" outlineLevel="2">
       <c r="E7" s="1" t="s">
         <v>71</v>
       </c>
@@ -3231,7 +3239,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="41.4" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="45" outlineLevel="2">
       <c r="E8" s="1" t="s">
         <v>75</v>
       </c>
@@ -3242,7 +3250,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="41.4" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="45" outlineLevel="2">
       <c r="E9" s="1" t="s">
         <v>73</v>
       </c>
@@ -3253,12 +3261,12 @@
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" outlineLevel="1">
       <c r="D10" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="2:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" outlineLevel="2">
       <c r="E11" s="1" t="s">
         <v>85</v>
       </c>
@@ -3266,7 +3274,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="41.4" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" ht="45" outlineLevel="2">
       <c r="E12" s="1" t="s">
         <v>83</v>
       </c>
@@ -3277,7 +3285,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="2:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" outlineLevel="2">
       <c r="E13" s="1" t="s">
         <v>18</v>
       </c>
@@ -3288,7 +3296,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="14" spans="2:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" outlineLevel="2">
       <c r="E14" s="1" t="s">
         <v>79</v>
       </c>
@@ -3299,7 +3307,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="2:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" outlineLevel="2">
       <c r="E15" s="1" t="s">
         <v>81</v>
       </c>
@@ -3310,7 +3318,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="2:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" outlineLevel="2">
       <c r="E16" s="1" t="s">
         <v>104</v>
       </c>
@@ -3318,7 +3326,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="17" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:7" outlineLevel="2">
       <c r="E17" s="1" t="s">
         <v>105</v>
       </c>
@@ -3326,13 +3334,13 @@
         <v>214</v>
       </c>
     </row>
-    <row r="18" spans="4:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:7" outlineLevel="1">
       <c r="D18" s="1" t="s">
         <v>89</v>
       </c>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:7" outlineLevel="2">
       <c r="E19" s="1" t="s">
         <v>92</v>
       </c>
@@ -3340,7 +3348,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="20" spans="4:7" ht="41.4" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:7" ht="45" outlineLevel="2">
       <c r="E20" s="1" t="s">
         <v>91</v>
       </c>
@@ -3351,7 +3359,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="21" spans="4:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:7" outlineLevel="1">
       <c r="D21" s="1" t="s">
         <v>87</v>
       </c>
@@ -3359,7 +3367,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="22" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:7" outlineLevel="2">
       <c r="E22" s="1" t="s">
         <v>95</v>
       </c>
@@ -3367,7 +3375,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="23" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:7" outlineLevel="2">
       <c r="E23" s="1" t="s">
         <v>93</v>
       </c>
@@ -3375,7 +3383,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="24" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:7" outlineLevel="2">
       <c r="E24" s="1" t="s">
         <v>94</v>
       </c>
@@ -3383,7 +3391,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="25" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:7" outlineLevel="2">
       <c r="E25" s="1" t="s">
         <v>105</v>
       </c>
@@ -3391,12 +3399,12 @@
         <v>214</v>
       </c>
     </row>
-    <row r="26" spans="4:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:7" outlineLevel="1">
       <c r="D26" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:7" outlineLevel="2">
       <c r="E27" s="1" t="s">
         <v>86</v>
       </c>
@@ -3404,7 +3412,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="28" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:7" outlineLevel="2">
       <c r="E28" s="1" t="s">
         <v>88</v>
       </c>
@@ -3412,12 +3420,12 @@
         <v>214</v>
       </c>
     </row>
-    <row r="29" spans="4:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:7" outlineLevel="1">
       <c r="D29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:7" outlineLevel="2">
       <c r="E30" s="1" t="s">
         <v>96</v>
       </c>
@@ -3425,7 +3433,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="31" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:7" outlineLevel="2">
       <c r="E31" s="1" t="s">
         <v>97</v>
       </c>
@@ -3433,7 +3441,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="32" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:7" outlineLevel="2">
       <c r="E32" s="1" t="s">
         <v>98</v>
       </c>
@@ -3441,7 +3449,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="33" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:7" outlineLevel="2">
       <c r="E33" s="1" t="s">
         <v>99</v>
       </c>
@@ -3449,7 +3457,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="34" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:7" outlineLevel="2">
       <c r="E34" s="1" t="s">
         <v>100</v>
       </c>
@@ -3457,7 +3465,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="35" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:7" outlineLevel="2">
       <c r="E35" s="1" t="s">
         <v>101</v>
       </c>
@@ -3465,7 +3473,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="36" spans="4:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:7" outlineLevel="1">
       <c r="D36" s="1" t="s">
         <v>31</v>
       </c>
@@ -3473,7 +3481,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="37" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:7" outlineLevel="2">
       <c r="E37" s="1" t="s">
         <v>102</v>
       </c>
@@ -3481,7 +3489,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="38" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:7" outlineLevel="2">
       <c r="E38" s="1" t="s">
         <v>103</v>
       </c>
@@ -3489,7 +3497,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="39" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:7" outlineLevel="2">
       <c r="E39" s="1" t="s">
         <v>105</v>
       </c>
@@ -3497,7 +3505,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="40" spans="4:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:7" outlineLevel="1">
       <c r="D40" s="1" t="s">
         <v>32</v>
       </c>
@@ -3505,7 +3513,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="41" spans="4:7" ht="41.4" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:7" ht="45" outlineLevel="2">
       <c r="E41" s="1" t="s">
         <v>108</v>
       </c>
@@ -3516,7 +3524,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="42" spans="4:7" ht="69" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:7" ht="75" outlineLevel="2">
       <c r="E42" s="1" t="s">
         <v>110</v>
       </c>
@@ -3527,7 +3535,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="43" spans="4:7" ht="27.6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:7" ht="30" outlineLevel="2">
       <c r="E43" s="1" t="s">
         <v>106</v>
       </c>
@@ -3538,7 +3546,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="44" spans="4:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:7" outlineLevel="1">
       <c r="D44" s="1" t="s">
         <v>33</v>
       </c>
@@ -3546,12 +3554,12 @@
         <v>207</v>
       </c>
     </row>
-    <row r="45" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:7" outlineLevel="2">
       <c r="E45" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:7" outlineLevel="2">
       <c r="E46" s="1" t="s">
         <v>124</v>
       </c>
@@ -3559,7 +3567,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="47" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:7" outlineLevel="2">
       <c r="E47" s="1" t="s">
         <v>122</v>
       </c>
@@ -3567,7 +3575,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="48" spans="4:7" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:7" outlineLevel="3">
       <c r="F48" s="1" t="s">
         <v>107</v>
       </c>
@@ -3575,7 +3583,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="49" spans="4:8" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:8" outlineLevel="3">
       <c r="F49" s="1" t="s">
         <v>113</v>
       </c>
@@ -3583,7 +3591,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="50" spans="4:8" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:8" outlineLevel="3">
       <c r="F50" s="1" t="s">
         <v>114</v>
       </c>
@@ -3591,7 +3599,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="51" spans="4:8" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:8" outlineLevel="3">
       <c r="F51" s="1" t="s">
         <v>115</v>
       </c>
@@ -3599,7 +3607,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="52" spans="4:8" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:8" outlineLevel="3">
       <c r="F52" s="1" t="s">
         <v>253</v>
       </c>
@@ -3607,7 +3615,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="53" spans="4:8" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:8" outlineLevel="3">
       <c r="F53" s="1" t="s">
         <v>254</v>
       </c>
@@ -3615,7 +3623,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="54" spans="4:8" ht="27.6" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:8" ht="30" outlineLevel="3">
       <c r="F54" s="1" t="s">
         <v>116</v>
       </c>
@@ -3626,7 +3634,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="55" spans="4:8" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:8" outlineLevel="3">
       <c r="F55" s="1" t="s">
         <v>256</v>
       </c>
@@ -3635,7 +3643,7 @@
       </c>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="4:8" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:8" outlineLevel="3">
       <c r="E56" s="1" t="s">
         <v>179</v>
       </c>
@@ -3643,7 +3651,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="57" spans="4:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:8" outlineLevel="1">
       <c r="D57" s="1" t="s">
         <v>118</v>
       </c>
@@ -3651,7 +3659,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="58" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:8" outlineLevel="2">
       <c r="E58" s="1" t="s">
         <v>125</v>
       </c>
@@ -3659,7 +3667,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:8" outlineLevel="2">
       <c r="E59" s="1" t="s">
         <v>126</v>
       </c>
@@ -3667,7 +3675,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="60" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:8" outlineLevel="2">
       <c r="E60" s="1" t="s">
         <v>127</v>
       </c>
@@ -3675,7 +3683,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="61" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:8" outlineLevel="2">
       <c r="E61" s="1" t="s">
         <v>128</v>
       </c>
@@ -3683,7 +3691,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="62" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:8" outlineLevel="2">
       <c r="E62" s="1" t="s">
         <v>257</v>
       </c>
@@ -3691,7 +3699,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="63" spans="4:8" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:8" outlineLevel="2">
       <c r="E63" s="1" t="s">
         <v>258</v>
       </c>
@@ -3699,12 +3707,12 @@
         <v>215</v>
       </c>
     </row>
-    <row r="64" spans="4:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:8" outlineLevel="1">
       <c r="D64" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="65" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:7" outlineLevel="2">
       <c r="E65" s="1" t="s">
         <v>129</v>
       </c>
@@ -3712,7 +3720,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="66" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:7" outlineLevel="2">
       <c r="E66" s="1" t="s">
         <v>259</v>
       </c>
@@ -3723,17 +3731,17 @@
         <v>261</v>
       </c>
     </row>
-    <row r="67" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:7" outlineLevel="2">
       <c r="E67" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:7" outlineLevel="2">
       <c r="E68" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="69" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:7" outlineLevel="2">
       <c r="E69" s="1" t="s">
         <v>133</v>
       </c>
@@ -3741,37 +3749,37 @@
         <v>132</v>
       </c>
     </row>
-    <row r="70" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:7" outlineLevel="2">
       <c r="E70" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="71" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:7" outlineLevel="2">
       <c r="E71" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="72" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:7" outlineLevel="2">
       <c r="E72" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="73" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:7" outlineLevel="2">
       <c r="E73" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="74" spans="4:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:7" outlineLevel="1">
       <c r="D74" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="75" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:7" outlineLevel="2">
       <c r="E75" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="76" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:7" outlineLevel="2">
       <c r="E76" s="1" t="s">
         <v>151</v>
       </c>
@@ -3779,257 +3787,257 @@
         <v>150</v>
       </c>
     </row>
-    <row r="77" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:7" outlineLevel="2">
       <c r="E77" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="78" spans="4:7" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:7" outlineLevel="3">
       <c r="F78" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="79" spans="4:7" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:7" outlineLevel="3">
       <c r="F79" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="80" spans="4:7" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:7" outlineLevel="3">
       <c r="F80" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="81" spans="4:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:6" outlineLevel="1">
       <c r="D81" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="82" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:6" outlineLevel="2">
       <c r="E82" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="83" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:6" outlineLevel="2">
       <c r="E83" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="84" spans="4:6" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:6" outlineLevel="3">
       <c r="F84" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="85" spans="4:6" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:6" outlineLevel="3">
       <c r="F85" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="86" spans="4:6" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:6" outlineLevel="3">
       <c r="F86" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="87" spans="4:6" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:6" outlineLevel="3">
       <c r="F87" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="88" spans="4:6" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:6" outlineLevel="3">
       <c r="F88" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="89" spans="4:6" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:6" outlineLevel="3">
       <c r="F89" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="90" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:6" outlineLevel="2">
       <c r="E90" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="91" spans="4:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:6" outlineLevel="1">
       <c r="D91" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="92" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:6" outlineLevel="2">
       <c r="E92" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="93" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:6" outlineLevel="2">
       <c r="E93" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="94" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:6" outlineLevel="2">
       <c r="E94" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="95" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:6" outlineLevel="2">
       <c r="E95" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="96" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:6" outlineLevel="2">
       <c r="E96" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="97" spans="3:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:6" outlineLevel="1">
       <c r="D97" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="98" spans="3:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:6" outlineLevel="2">
       <c r="E98" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="99" spans="3:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:6" outlineLevel="2">
       <c r="E99" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="100" spans="3:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:6" outlineLevel="1">
       <c r="C100" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="101" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:6">
       <c r="C101" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="102" spans="3:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:6" outlineLevel="1">
       <c r="D102" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="103" spans="3:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:6" outlineLevel="2">
       <c r="E103" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="104" spans="3:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:6" outlineLevel="2">
       <c r="E104" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="105" spans="3:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:6" outlineLevel="2">
       <c r="E105" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="106" spans="3:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:6" outlineLevel="2">
       <c r="E106" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="107" spans="3:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:6" outlineLevel="2">
       <c r="F107" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="108" spans="3:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:6" outlineLevel="2">
       <c r="F108" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="109" spans="3:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:6" outlineLevel="2">
       <c r="F109" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="110" spans="3:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:6" outlineLevel="2">
       <c r="E110" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="111" spans="3:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:6" outlineLevel="2">
       <c r="E111" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="112" spans="3:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:6" outlineLevel="2">
       <c r="E112" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="113" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="113" spans="4:6" outlineLevel="2">
       <c r="E113" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="114" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="114" spans="4:6" outlineLevel="2">
       <c r="E114" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="115" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="115" spans="4:6" outlineLevel="2">
       <c r="E115" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="116" spans="4:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="4:6" outlineLevel="1">
       <c r="D116" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="117" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="117" spans="4:6" outlineLevel="2">
       <c r="E117" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="118" spans="4:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="4:6" outlineLevel="1">
       <c r="D118" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="119" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="119" spans="4:6" outlineLevel="2">
       <c r="E119" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="120" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="120" spans="4:6" outlineLevel="2">
       <c r="F120" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="121" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="121" spans="4:6" outlineLevel="2">
       <c r="F121" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="122" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="122" spans="4:6" outlineLevel="2">
       <c r="E122" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="123" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="123" spans="4:6" outlineLevel="2">
       <c r="F123" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="124" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="124" spans="4:6" outlineLevel="2">
       <c r="F124" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="125" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="125" spans="4:6" outlineLevel="2">
       <c r="F125" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="126" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="126" spans="4:6" outlineLevel="2">
       <c r="E126" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="127" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="127" spans="4:6" outlineLevel="2">
       <c r="E127" s="1" t="s">
         <v>231</v>
       </c>
@@ -4037,7 +4045,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="128" spans="4:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="128" spans="4:6" outlineLevel="2">
       <c r="E128" s="1" t="s">
         <v>232</v>
       </c>
@@ -4045,7 +4053,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="129" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" outlineLevel="2">
       <c r="E129" s="1" t="s">
         <v>233</v>
       </c>
@@ -4053,27 +4061,27 @@
         <v>237</v>
       </c>
     </row>
-    <row r="130" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" outlineLevel="2">
       <c r="E130" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="131" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" outlineLevel="1">
       <c r="D131" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="132" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" outlineLevel="2">
       <c r="E132" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="133" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" outlineLevel="2">
       <c r="E133" s="1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="134" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" outlineLevel="1">
       <c r="D134" s="1" t="s">
         <v>582</v>
       </c>
@@ -4082,7 +4090,7 @@
       </c>
       <c r="G134" s="4"/>
     </row>
-    <row r="135" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" outlineLevel="2">
       <c r="E135" s="1" t="s">
         <v>221</v>
       </c>
@@ -4091,7 +4099,7 @@
       </c>
       <c r="G135" s="4"/>
     </row>
-    <row r="136" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" outlineLevel="2">
       <c r="E136" s="1" t="s">
         <v>239</v>
       </c>
@@ -4100,7 +4108,7 @@
       </c>
       <c r="G136" s="4"/>
     </row>
-    <row r="137" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" outlineLevel="2">
       <c r="A137" s="1" t="s">
         <v>238</v>
       </c>
@@ -4109,25 +4117,25 @@
       </c>
       <c r="G137" s="4"/>
     </row>
-    <row r="138" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" outlineLevel="2">
       <c r="E138" s="1" t="s">
         <v>250</v>
       </c>
       <c r="G138" s="4"/>
     </row>
-    <row r="139" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" outlineLevel="2">
       <c r="E139" s="1" t="s">
         <v>195</v>
       </c>
       <c r="G139" s="4"/>
     </row>
-    <row r="140" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" outlineLevel="2">
       <c r="F140" s="1" t="s">
         <v>244</v>
       </c>
       <c r="G140" s="4"/>
     </row>
-    <row r="141" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" outlineLevel="2">
       <c r="A141" s="1" t="s">
         <v>238</v>
       </c>
@@ -4136,7 +4144,7 @@
       </c>
       <c r="G141" s="4"/>
     </row>
-    <row r="142" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" outlineLevel="2">
       <c r="A142" s="1" t="s">
         <v>238</v>
       </c>
@@ -4145,31 +4153,31 @@
       </c>
       <c r="G142" s="4"/>
     </row>
-    <row r="143" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" outlineLevel="2">
       <c r="E143" s="1" t="s">
         <v>196</v>
       </c>
       <c r="G143" s="4"/>
     </row>
-    <row r="144" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" outlineLevel="2">
       <c r="F144" s="1" t="s">
         <v>251</v>
       </c>
       <c r="G144" s="4"/>
     </row>
-    <row r="145" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" outlineLevel="2">
       <c r="F145" s="1" t="s">
         <v>252</v>
       </c>
       <c r="G145" s="4"/>
     </row>
-    <row r="146" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" outlineLevel="2">
       <c r="F146" s="1" t="s">
         <v>204</v>
       </c>
       <c r="G146" s="4"/>
     </row>
-    <row r="147" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" outlineLevel="1">
       <c r="A147" s="1" t="s">
         <v>238</v>
       </c>
@@ -4178,43 +4186,43 @@
       </c>
       <c r="G147" s="4"/>
     </row>
-    <row r="148" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" outlineLevel="2">
       <c r="E148" s="1" t="s">
         <v>249</v>
       </c>
       <c r="G148" s="4"/>
     </row>
-    <row r="149" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" outlineLevel="2">
       <c r="E149" s="1" t="s">
         <v>222</v>
       </c>
       <c r="G149" s="4"/>
     </row>
-    <row r="150" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" outlineLevel="1">
       <c r="D150" s="1" t="s">
         <v>190</v>
       </c>
       <c r="G150" s="4"/>
     </row>
-    <row r="151" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" outlineLevel="2">
       <c r="E151" s="1" t="s">
         <v>249</v>
       </c>
       <c r="G151" s="4"/>
     </row>
-    <row r="152" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" outlineLevel="2">
       <c r="E152" s="1" t="s">
         <v>222</v>
       </c>
       <c r="G152" s="4"/>
     </row>
-    <row r="153" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" outlineLevel="1">
       <c r="G153" s="4"/>
     </row>
-    <row r="154" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" outlineLevel="1">
       <c r="G154" s="4"/>
     </row>
-    <row r="155" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" outlineLevel="1">
       <c r="C155" s="3" t="s">
         <v>55</v>
       </c>
@@ -4232,34 +4240,34 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L266"/>
+  <dimension ref="A1:L269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A245" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F267" sqref="F267"/>
+    <sheetView tabSelected="1" topLeftCell="A242" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G269" sqref="G269"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="23.44140625" customWidth="1"/>
-    <col min="7" max="7" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.21875" customWidth="1"/>
-    <col min="9" max="9" width="42.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="55.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="51.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="51.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -4267,7 +4275,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
@@ -4275,7 +4283,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:7" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" collapsed="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
@@ -4283,7 +4291,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" hidden="1" outlineLevel="1">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
@@ -4292,7 +4300,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" hidden="1" outlineLevel="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
@@ -4301,7 +4309,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" outlineLevel="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
@@ -4310,7 +4318,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" hidden="1" outlineLevel="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
@@ -4322,7 +4330,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" outlineLevel="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
@@ -4334,7 +4342,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" hidden="1" outlineLevel="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
@@ -4346,7 +4354,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" hidden="1" outlineLevel="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
@@ -4355,7 +4363,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" hidden="1" outlineLevel="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
@@ -4364,7 +4372,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" hidden="1" outlineLevel="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
@@ -4376,7 +4384,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" hidden="1" outlineLevel="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
@@ -4385,7 +4393,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" hidden="1" outlineLevel="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
@@ -4394,7 +4402,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" outlineLevel="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
@@ -4403,7 +4411,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" hidden="1" outlineLevel="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
@@ -4411,7 +4419,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -4419,7 +4427,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="19" spans="1:7" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" outlineLevel="1" collapsed="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -4428,7 +4436,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" hidden="1" outlineLevel="2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -4440,7 +4448,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" hidden="1" outlineLevel="2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -4449,13 +4457,13 @@
         <v>394</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" hidden="1" outlineLevel="2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" hidden="1" outlineLevel="2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -4464,7 +4472,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" hidden="1" outlineLevel="2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -4473,7 +4481,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" hidden="1" outlineLevel="2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -4482,7 +4490,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" hidden="1" outlineLevel="2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -4491,13 +4499,13 @@
         <v>409</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" hidden="1" outlineLevel="2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" hidden="1" outlineLevel="2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -4506,7 +4514,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" hidden="1" outlineLevel="2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -4515,7 +4523,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" hidden="1" outlineLevel="2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -4524,7 +4532,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" hidden="1" outlineLevel="2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -4533,7 +4541,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" hidden="1" outlineLevel="2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -4542,7 +4550,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" hidden="1" outlineLevel="2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -4551,7 +4559,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" hidden="1" outlineLevel="2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -4560,7 +4568,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" hidden="1" outlineLevel="2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -4569,7 +4577,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" hidden="1" outlineLevel="2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -4578,18 +4586,18 @@
         <v>336</v>
       </c>
     </row>
-    <row r="37" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" outlineLevel="1" collapsed="1">
       <c r="E37" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" hidden="1" outlineLevel="2">
       <c r="F38" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" hidden="1" outlineLevel="2"/>
+    <row r="40" spans="1:12" hidden="1" outlineLevel="2">
       <c r="F40" t="s">
         <v>292</v>
       </c>
@@ -4612,7 +4620,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" hidden="1" outlineLevel="2">
       <c r="F41" t="s">
         <v>313</v>
       </c>
@@ -4632,7 +4640,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" hidden="1" outlineLevel="2">
       <c r="F42" t="s">
         <v>314</v>
       </c>
@@ -4652,7 +4660,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" hidden="1" outlineLevel="2">
       <c r="F43" t="s">
         <v>315</v>
       </c>
@@ -4672,7 +4680,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" hidden="1" outlineLevel="2">
       <c r="F44" t="s">
         <v>316</v>
       </c>
@@ -4692,7 +4700,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" hidden="1" outlineLevel="2">
       <c r="F45" t="s">
         <v>317</v>
       </c>
@@ -4712,7 +4720,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" hidden="1" outlineLevel="2">
       <c r="F46" t="s">
         <v>318</v>
       </c>
@@ -4732,7 +4740,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" hidden="1" outlineLevel="2">
       <c r="F47" t="s">
         <v>319</v>
       </c>
@@ -4749,7 +4757,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" hidden="1" outlineLevel="2">
       <c r="F48" t="s">
         <v>320</v>
       </c>
@@ -4769,7 +4777,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="49" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="49" spans="6:12" hidden="1" outlineLevel="2">
       <c r="F49" t="s">
         <v>321</v>
       </c>
@@ -4789,7 +4797,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="50" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="50" spans="6:12" hidden="1" outlineLevel="2">
       <c r="F50" t="s">
         <v>323</v>
       </c>
@@ -4809,7 +4817,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="51" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="51" spans="6:12" hidden="1" outlineLevel="2">
       <c r="F51" t="s">
         <v>322</v>
       </c>
@@ -4829,7 +4837,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="52" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="52" spans="6:12" hidden="1" outlineLevel="2">
       <c r="F52" t="s">
         <v>324</v>
       </c>
@@ -4849,7 +4857,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="53" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="53" spans="6:12" hidden="1" outlineLevel="2">
       <c r="F53" t="s">
         <v>325</v>
       </c>
@@ -4869,7 +4877,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="54" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="54" spans="6:12" hidden="1" outlineLevel="2">
       <c r="F54" t="s">
         <v>326</v>
       </c>
@@ -4886,7 +4894,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="55" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="55" spans="6:12" hidden="1" outlineLevel="2">
       <c r="F55" t="s">
         <v>327</v>
       </c>
@@ -4903,7 +4911,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="56" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="56" spans="6:12" hidden="1" outlineLevel="2">
       <c r="F56" t="s">
         <v>328</v>
       </c>
@@ -4920,7 +4928,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="57" spans="6:12" ht="27.6" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="57" spans="6:12" ht="30" hidden="1" outlineLevel="2">
       <c r="F57" t="s">
         <v>329</v>
       </c>
@@ -4940,7 +4948,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="58" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="58" spans="6:12" hidden="1" outlineLevel="2">
       <c r="F58" t="s">
         <v>330</v>
       </c>
@@ -4960,7 +4968,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="59" spans="6:12" hidden="1" outlineLevel="2">
       <c r="F59" t="s">
         <v>331</v>
       </c>
@@ -4980,7 +4988,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="60" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="60" spans="6:12" hidden="1" outlineLevel="2">
       <c r="F60" t="s">
         <v>332</v>
       </c>
@@ -5000,7 +5008,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="61" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="61" spans="6:12" hidden="1" outlineLevel="2">
       <c r="F61" t="s">
         <v>333</v>
       </c>
@@ -5017,7 +5025,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="62" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="62" spans="6:12" hidden="1" outlineLevel="2">
       <c r="F62" t="s">
         <v>334</v>
       </c>
@@ -5034,7 +5042,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="63" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="63" spans="6:12" hidden="1" outlineLevel="2">
       <c r="F63" t="s">
         <v>335</v>
       </c>
@@ -5051,8 +5059,8 @@
         <v>214</v>
       </c>
     </row>
-    <row r="64" spans="6:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="64" spans="6:12" hidden="1" outlineLevel="2"/>
+    <row r="65" spans="5:12" hidden="1" outlineLevel="2">
       <c r="F65" t="s">
         <v>535</v>
       </c>
@@ -5072,7 +5080,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="66" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="66" spans="5:12" hidden="1" outlineLevel="2">
       <c r="F66" t="s">
         <v>529</v>
       </c>
@@ -5092,7 +5100,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="67" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="67" spans="5:12" hidden="1" outlineLevel="2">
       <c r="F67" t="s">
         <v>532</v>
       </c>
@@ -5112,7 +5120,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="68" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="68" spans="5:12" hidden="1" outlineLevel="2">
       <c r="F68" t="s">
         <v>533</v>
       </c>
@@ -5129,8 +5137,8 @@
         <v>573</v>
       </c>
     </row>
-    <row r="69" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="69" spans="5:12" hidden="1" outlineLevel="2"/>
+    <row r="70" spans="5:12" hidden="1" outlineLevel="2">
       <c r="F70" t="s">
         <v>544</v>
       </c>
@@ -5150,7 +5158,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="71" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:12" hidden="1" outlineLevel="2">
       <c r="F71" t="s">
         <v>545</v>
       </c>
@@ -5170,7 +5178,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="72" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:12" hidden="1" outlineLevel="2">
       <c r="F72" t="s">
         <v>547</v>
       </c>
@@ -5190,7 +5198,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="73" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="73" spans="5:12" hidden="1" outlineLevel="2">
       <c r="F73" t="s">
         <v>546</v>
       </c>
@@ -5210,7 +5218,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="74" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="74" spans="5:12" hidden="1" outlineLevel="2">
       <c r="F74" t="s">
         <v>548</v>
       </c>
@@ -5230,7 +5238,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="75" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="75" spans="5:12" hidden="1" outlineLevel="2">
       <c r="F75" t="s">
         <v>550</v>
       </c>
@@ -5250,24 +5258,24 @@
         <v>573</v>
       </c>
     </row>
-    <row r="76" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="76" spans="5:12" hidden="1" outlineLevel="2"/>
+    <row r="77" spans="5:12" hidden="1" outlineLevel="2">
       <c r="E77" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="78" spans="5:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="5:12" outlineLevel="1" collapsed="1">
       <c r="E78" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="79" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="79" spans="5:12" hidden="1" outlineLevel="2">
       <c r="F79" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="80" spans="5:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25"/>
-    <row r="81" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="80" spans="5:12" hidden="1" outlineLevel="2"/>
+    <row r="81" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G81" t="s">
         <v>265</v>
       </c>
@@ -5284,7 +5292,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="82" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="82" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G82" t="s">
         <v>268</v>
       </c>
@@ -5298,7 +5306,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="83" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="83" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G83" t="s">
         <v>269</v>
       </c>
@@ -5312,7 +5320,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="84" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="84" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G84" t="s">
         <v>271</v>
       </c>
@@ -5326,7 +5334,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="85" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="85" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G85" t="s">
         <v>281</v>
       </c>
@@ -5340,7 +5348,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="86" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="86" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G86" t="s">
         <v>283</v>
       </c>
@@ -5354,7 +5362,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="87" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="87" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G87" t="s">
         <v>284</v>
       </c>
@@ -5368,7 +5376,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="88" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="88" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G88" t="s">
         <v>286</v>
       </c>
@@ -5382,7 +5390,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="89" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="89" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G89" t="s">
         <v>287</v>
       </c>
@@ -5396,7 +5404,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="90" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="90" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G90" t="s">
         <v>288</v>
       </c>
@@ -5410,7 +5418,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="91" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="91" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G91" t="s">
         <v>289</v>
       </c>
@@ -5424,7 +5432,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="92" spans="7:11" ht="41.4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="92" spans="7:11" ht="45" hidden="1" outlineLevel="2">
       <c r="G92" t="s">
         <v>291</v>
       </c>
@@ -5438,7 +5446,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="93" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="93" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G93" t="s">
         <v>293</v>
       </c>
@@ -5452,7 +5460,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="94" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="94" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G94" t="s">
         <v>295</v>
       </c>
@@ -5466,7 +5474,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="95" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="95" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G95" t="s">
         <v>296</v>
       </c>
@@ -5480,7 +5488,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="96" spans="7:11" ht="27.6" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="96" spans="7:11" ht="30" hidden="1" outlineLevel="2">
       <c r="G96" t="s">
         <v>298</v>
       </c>
@@ -5494,7 +5502,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="97" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="97" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G97" t="s">
         <v>300</v>
       </c>
@@ -5508,7 +5516,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="98" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="98" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G98" t="s">
         <v>301</v>
       </c>
@@ -5522,7 +5530,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="99" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="99" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G99" t="s">
         <v>304</v>
       </c>
@@ -5536,7 +5544,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="100" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="100" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G100" t="s">
         <v>305</v>
       </c>
@@ -5550,10 +5558,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="101" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="101" spans="7:11" hidden="1" outlineLevel="2">
       <c r="I101" s="5"/>
     </row>
-    <row r="102" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="102" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G102" t="s">
         <v>526</v>
       </c>
@@ -5567,7 +5575,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="103" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="103" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G103" t="s">
         <v>525</v>
       </c>
@@ -5581,7 +5589,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="104" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="104" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G104" t="s">
         <v>528</v>
       </c>
@@ -5595,7 +5603,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="105" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="105" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G105" t="s">
         <v>527</v>
       </c>
@@ -5609,10 +5617,10 @@
         <v>573</v>
       </c>
     </row>
-    <row r="106" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="106" spans="7:11" hidden="1" outlineLevel="2">
       <c r="I106" s="5"/>
     </row>
-    <row r="107" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="107" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G107" t="s">
         <v>540</v>
       </c>
@@ -5626,7 +5634,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="108" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="108" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G108" t="s">
         <v>541</v>
       </c>
@@ -5640,7 +5648,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="109" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="109" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G109" t="s">
         <v>543</v>
       </c>
@@ -5654,7 +5662,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="110" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="110" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G110" t="s">
         <v>542</v>
       </c>
@@ -5668,7 +5676,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="111" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="111" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G111" t="s">
         <v>549</v>
       </c>
@@ -5682,7 +5690,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="112" spans="7:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="112" spans="7:11" hidden="1" outlineLevel="2">
       <c r="G112" t="s">
         <v>551</v>
       </c>
@@ -5696,10 +5704,10 @@
         <v>573</v>
       </c>
     </row>
-    <row r="113" spans="4:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="113" spans="4:11" hidden="1" outlineLevel="2">
       <c r="I113" s="5"/>
     </row>
-    <row r="114" spans="4:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="114" spans="4:11" hidden="1" outlineLevel="2">
       <c r="F114" t="s">
         <v>463</v>
       </c>
@@ -5708,27 +5716,27 @@
         <v>464</v>
       </c>
     </row>
-    <row r="115" spans="4:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="115" spans="4:11" hidden="1" outlineLevel="2">
       <c r="E115" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="116" spans="4:11" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="4:11" outlineLevel="1" collapsed="1">
       <c r="E116" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="117" spans="4:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="117" spans="4:11" hidden="1" outlineLevel="2">
       <c r="E117" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="118" spans="4:11" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="4:11" outlineLevel="1" collapsed="1">
       <c r="E118" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="119" spans="4:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="119" spans="4:11" hidden="1" outlineLevel="2">
       <c r="G119" t="s">
         <v>265</v>
       </c>
@@ -5739,7 +5747,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="120" spans="4:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="120" spans="4:11" hidden="1" outlineLevel="2">
       <c r="G120" t="s">
         <v>276</v>
       </c>
@@ -5750,7 +5758,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="121" spans="4:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="121" spans="4:11" hidden="1" outlineLevel="2">
       <c r="E121" t="s">
         <v>336</v>
       </c>
@@ -5764,23 +5772,23 @@
         <v>215</v>
       </c>
     </row>
-    <row r="122" spans="4:11" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="4:11" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="4:11" outlineLevel="1"/>
+    <row r="123" spans="4:11" outlineLevel="1">
       <c r="D123" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="124" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="4:11">
       <c r="D124" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="125" spans="4:11" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="4:11" outlineLevel="1" collapsed="1">
       <c r="E125" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="126" spans="4:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="126" spans="4:11" hidden="1" outlineLevel="2">
       <c r="F126" t="s">
         <v>480</v>
       </c>
@@ -5788,28 +5796,28 @@
         <v>405</v>
       </c>
     </row>
-    <row r="127" spans="4:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="127" spans="4:11" hidden="1" outlineLevel="2">
       <c r="F127" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="128" spans="4:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25"/>
-    <row r="129" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="128" spans="4:11" hidden="1" outlineLevel="2"/>
+    <row r="129" spans="5:9" hidden="1" outlineLevel="2">
       <c r="F129" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="130" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="130" spans="5:9" hidden="1" outlineLevel="2">
       <c r="G130" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="131" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="131" spans="5:9" hidden="1" outlineLevel="2">
       <c r="G131" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="132" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="132" spans="5:9" hidden="1" outlineLevel="2">
       <c r="G132" t="s">
         <v>420</v>
       </c>
@@ -5817,7 +5825,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="133" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="133" spans="5:9" hidden="1" outlineLevel="2">
       <c r="G133" t="s">
         <v>421</v>
       </c>
@@ -5825,7 +5833,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="134" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="134" spans="5:9" hidden="1" outlineLevel="2">
       <c r="G134" t="s">
         <v>422</v>
       </c>
@@ -5833,7 +5841,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="135" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="135" spans="5:9" hidden="1" outlineLevel="2">
       <c r="G135" t="s">
         <v>423</v>
       </c>
@@ -5841,7 +5849,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="136" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="136" spans="5:9" hidden="1" outlineLevel="2">
       <c r="G136" t="s">
         <v>424</v>
       </c>
@@ -5849,7 +5857,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="137" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="137" spans="5:9" hidden="1" outlineLevel="2">
       <c r="G137" t="s">
         <v>425</v>
       </c>
@@ -5857,7 +5865,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="138" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="138" spans="5:9" hidden="1" outlineLevel="2">
       <c r="G138" t="s">
         <v>432</v>
       </c>
@@ -5865,17 +5873,17 @@
         <v>433</v>
       </c>
     </row>
-    <row r="139" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="139" spans="5:9" hidden="1" outlineLevel="2">
       <c r="G139" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="140" spans="5:9" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="5:9" outlineLevel="1" collapsed="1">
       <c r="E140" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="141" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="141" spans="5:9" hidden="1" outlineLevel="2">
       <c r="F141" t="s">
         <v>435</v>
       </c>
@@ -5886,7 +5894,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="142" spans="5:9" ht="55.2" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="142" spans="5:9" ht="75" hidden="1" outlineLevel="2">
       <c r="F142" t="s">
         <v>442</v>
       </c>
@@ -5897,7 +5905,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="143" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="143" spans="5:9" hidden="1" outlineLevel="2">
       <c r="F143" t="s">
         <v>443</v>
       </c>
@@ -5908,7 +5916,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="144" spans="5:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="144" spans="5:9" hidden="1" outlineLevel="2">
       <c r="F144" t="s">
         <v>444</v>
       </c>
@@ -5916,7 +5924,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="145" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="145" spans="6:9" hidden="1" outlineLevel="2">
       <c r="F145" t="s">
         <v>445</v>
       </c>
@@ -5927,7 +5935,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="146" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="146" spans="6:9" hidden="1" outlineLevel="2">
       <c r="F146" t="s">
         <v>436</v>
       </c>
@@ -5938,7 +5946,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="147" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="147" spans="6:9" hidden="1" outlineLevel="2">
       <c r="F147" t="s">
         <v>437</v>
       </c>
@@ -5949,7 +5957,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="148" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="148" spans="6:9" hidden="1" outlineLevel="2">
       <c r="F148" t="s">
         <v>438</v>
       </c>
@@ -5957,7 +5965,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="149" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="149" spans="6:9" hidden="1" outlineLevel="2">
       <c r="F149" t="s">
         <v>439</v>
       </c>
@@ -5965,7 +5973,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="150" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="150" spans="6:9" hidden="1" outlineLevel="2">
       <c r="F150" t="s">
         <v>440</v>
       </c>
@@ -5973,7 +5981,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="151" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="151" spans="6:9" hidden="1" outlineLevel="2">
       <c r="F151" t="s">
         <v>441</v>
       </c>
@@ -5981,7 +5989,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="152" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="152" spans="6:9" hidden="1" outlineLevel="2">
       <c r="F152" t="s">
         <v>446</v>
       </c>
@@ -5989,7 +5997,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="153" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="153" spans="6:9" hidden="1" outlineLevel="2">
       <c r="F153" t="s">
         <v>447</v>
       </c>
@@ -5997,7 +6005,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="154" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="154" spans="6:9" hidden="1" outlineLevel="2">
       <c r="F154" t="s">
         <v>448</v>
       </c>
@@ -6005,7 +6013,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="155" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="155" spans="6:9" hidden="1" outlineLevel="2">
       <c r="F155" t="s">
         <v>449</v>
       </c>
@@ -6013,7 +6021,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="156" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="156" spans="6:9" hidden="1" outlineLevel="2">
       <c r="F156" t="s">
         <v>450</v>
       </c>
@@ -6021,7 +6029,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="157" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="157" spans="6:9" hidden="1" outlineLevel="2">
       <c r="F157" t="s">
         <v>451</v>
       </c>
@@ -6029,7 +6037,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="158" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="158" spans="6:9" hidden="1" outlineLevel="2">
       <c r="F158" t="s">
         <v>317</v>
       </c>
@@ -6037,7 +6045,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="159" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="159" spans="6:9" hidden="1" outlineLevel="2">
       <c r="F159" t="s">
         <v>452</v>
       </c>
@@ -6045,7 +6053,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="160" spans="6:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="160" spans="6:9" hidden="1" outlineLevel="2">
       <c r="F160" t="s">
         <v>453</v>
       </c>
@@ -6053,7 +6061,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="161" spans="4:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="161" spans="4:9" hidden="1" outlineLevel="2">
       <c r="F161" t="s">
         <v>454</v>
       </c>
@@ -6061,7 +6069,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="162" spans="4:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="162" spans="4:9" hidden="1" outlineLevel="2">
       <c r="F162" t="s">
         <v>455</v>
       </c>
@@ -6069,7 +6077,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="163" spans="4:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="163" spans="4:9" hidden="1" outlineLevel="2">
       <c r="F163" t="s">
         <v>334</v>
       </c>
@@ -6077,7 +6085,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="164" spans="4:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="164" spans="4:9" hidden="1" outlineLevel="2">
       <c r="F164" t="s">
         <v>461</v>
       </c>
@@ -6088,29 +6096,29 @@
         <v>215</v>
       </c>
     </row>
-    <row r="165" spans="4:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25"/>
-    <row r="166" spans="4:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="165" spans="4:9" hidden="1" outlineLevel="2"/>
+    <row r="166" spans="4:9" hidden="1" outlineLevel="2">
       <c r="E166" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="167" spans="4:9" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="168" spans="4:9" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="4:9" outlineLevel="1"/>
+    <row r="168" spans="4:9" outlineLevel="1">
       <c r="D168" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="169" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="4:9">
       <c r="D169" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="170" spans="4:9" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="4:9" outlineLevel="1">
       <c r="E170" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="171" spans="4:9" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="4:9" outlineLevel="1">
       <c r="F171" t="s">
         <v>471</v>
       </c>
@@ -6118,28 +6126,28 @@
         <v>472</v>
       </c>
     </row>
-    <row r="172" spans="4:9" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="4:9" outlineLevel="1">
       <c r="F172" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="173" spans="4:9" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="174" spans="4:9" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="4:9" outlineLevel="1"/>
+    <row r="174" spans="4:9" outlineLevel="1">
       <c r="F174" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="175" spans="4:9" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="4:9" outlineLevel="1">
       <c r="G175" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="176" spans="4:9" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="4:9" outlineLevel="1">
       <c r="G176" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="177" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="5:8" outlineLevel="1">
       <c r="G177" t="s">
         <v>476</v>
       </c>
@@ -6147,7 +6155,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="178" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="5:8" outlineLevel="1">
       <c r="G178" t="s">
         <v>477</v>
       </c>
@@ -6155,7 +6163,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="179" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="5:8" outlineLevel="1">
       <c r="G179" t="s">
         <v>422</v>
       </c>
@@ -6163,7 +6171,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="180" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="5:8" outlineLevel="1">
       <c r="G180" t="s">
         <v>478</v>
       </c>
@@ -6171,7 +6179,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="181" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="5:8" outlineLevel="1">
       <c r="G181" t="s">
         <v>423</v>
       </c>
@@ -6179,7 +6187,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="182" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="5:8" outlineLevel="1">
       <c r="G182" t="s">
         <v>424</v>
       </c>
@@ -6187,7 +6195,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="183" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="5:8" outlineLevel="1">
       <c r="G183" t="s">
         <v>479</v>
       </c>
@@ -6195,7 +6203,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="184" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="5:8" outlineLevel="1">
       <c r="G184" t="s">
         <v>432</v>
       </c>
@@ -6203,60 +6211,60 @@
         <v>576</v>
       </c>
     </row>
-    <row r="185" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="5:8" outlineLevel="1">
       <c r="G185" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="186" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="187" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="5:8" outlineLevel="1"/>
+    <row r="187" spans="5:8" outlineLevel="1">
       <c r="E187" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="188" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="5:8" outlineLevel="1">
       <c r="F188" s="7" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="189" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="5:8" outlineLevel="1">
       <c r="F189" s="7"/>
       <c r="G189" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="190" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="5:8" outlineLevel="1">
       <c r="F190" s="7"/>
       <c r="G190" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="191" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="5:8" outlineLevel="1">
       <c r="F191" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="192" spans="5:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="5:8" outlineLevel="1">
       <c r="F192" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="193" spans="5:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="5:7" outlineLevel="1">
       <c r="F193" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="194" spans="5:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="5:7" outlineLevel="1">
       <c r="F194" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="195" spans="5:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="5:7" outlineLevel="1">
       <c r="E195" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="196" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="196" spans="5:7" outlineLevel="2">
       <c r="F196" t="s">
         <v>491</v>
       </c>
@@ -6264,7 +6272,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="197" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="197" spans="5:7" outlineLevel="2">
       <c r="F197" t="s">
         <v>489</v>
       </c>
@@ -6272,7 +6280,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="198" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="198" spans="5:7" outlineLevel="2">
       <c r="F198" t="s">
         <v>493</v>
       </c>
@@ -6280,8 +6288,8 @@
         <v>494</v>
       </c>
     </row>
-    <row r="199" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25"/>
-    <row r="200" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="199" spans="5:7" outlineLevel="2"/>
+    <row r="200" spans="5:7" outlineLevel="2">
       <c r="F200" t="s">
         <v>495</v>
       </c>
@@ -6289,7 +6297,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="201" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="201" spans="5:7" outlineLevel="2">
       <c r="F201" t="s">
         <v>499</v>
       </c>
@@ -6297,7 +6305,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="202" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="202" spans="5:7" outlineLevel="2">
       <c r="F202" t="s">
         <v>500</v>
       </c>
@@ -6305,7 +6313,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="203" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="203" spans="5:7" outlineLevel="2">
       <c r="F203" t="s">
         <v>501</v>
       </c>
@@ -6313,7 +6321,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="204" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="204" spans="5:7" outlineLevel="2">
       <c r="F204" t="s">
         <v>503</v>
       </c>
@@ -6321,7 +6329,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="205" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="205" spans="5:7" outlineLevel="2">
       <c r="F205" t="s">
         <v>505</v>
       </c>
@@ -6329,7 +6337,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="206" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="206" spans="5:7" outlineLevel="2">
       <c r="F206" t="s">
         <v>507</v>
       </c>
@@ -6337,7 +6345,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="207" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="207" spans="5:7" outlineLevel="2">
       <c r="F207" t="s">
         <v>509</v>
       </c>
@@ -6345,8 +6353,8 @@
         <v>510</v>
       </c>
     </row>
-    <row r="208" spans="5:7" outlineLevel="2" x14ac:dyDescent="0.25"/>
-    <row r="209" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="208" spans="5:7" outlineLevel="2"/>
+    <row r="209" spans="4:7" outlineLevel="2">
       <c r="F209" t="s">
         <v>511</v>
       </c>
@@ -6354,7 +6362,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="210" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="210" spans="4:7" outlineLevel="2">
       <c r="F210" t="s">
         <v>512</v>
       </c>
@@ -6362,7 +6370,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="211" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="211" spans="4:7" outlineLevel="2">
       <c r="F211" t="s">
         <v>515</v>
       </c>
@@ -6370,7 +6378,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="212" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="212" spans="4:7" outlineLevel="2">
       <c r="F212" t="s">
         <v>517</v>
       </c>
@@ -6378,7 +6386,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="213" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="213" spans="4:7" outlineLevel="2">
       <c r="F213" t="s">
         <v>519</v>
       </c>
@@ -6386,7 +6394,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="214" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="214" spans="4:7" outlineLevel="2">
       <c r="F214" t="s">
         <v>521</v>
       </c>
@@ -6394,7 +6402,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="215" spans="4:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="215" spans="4:7" outlineLevel="2">
       <c r="F215" t="s">
         <v>523</v>
       </c>
@@ -6402,130 +6410,145 @@
         <v>524</v>
       </c>
     </row>
-    <row r="216" spans="4:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="4:7" outlineLevel="1">
       <c r="E216" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="217" spans="4:7" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="218" spans="4:7" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="219" spans="4:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="4:7" outlineLevel="1"/>
+    <row r="218" spans="4:7" outlineLevel="1"/>
+    <row r="219" spans="4:7" outlineLevel="1">
       <c r="D219" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="221" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="4:7">
       <c r="D221" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="222" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="4:7">
       <c r="F222" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="227" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="6:6">
       <c r="F227" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="232" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="6:6">
       <c r="F232" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="242" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="4:7">
       <c r="D242" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="243" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="4:7">
       <c r="E243" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="244" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="4:7">
       <c r="F244" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="245" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="4:7">
       <c r="F245" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="246" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="4:7">
       <c r="F246" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="247" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="4:7">
       <c r="E247" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="248" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="4:7">
       <c r="F248" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="249" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="4:7">
       <c r="G249" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="250" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="4:7">
       <c r="G250" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="251" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="4:7">
       <c r="G251" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="253" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="4:7">
       <c r="F253" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="254" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="254" spans="4:7">
       <c r="G254" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="255" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="255" spans="4:7">
       <c r="G255" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:7">
       <c r="F259" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:7">
       <c r="G260" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:7">
       <c r="G261" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:7">
       <c r="A262" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:7">
       <c r="F263" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E266" t="s">
+    <row r="266" spans="1:7">
+      <c r="F266" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7">
+      <c r="G267" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7">
+      <c r="G268" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7">
+      <c r="E269" t="s">
         <v>601</v>
       </c>
     </row>

</xml_diff>